<commit_message>
Change to relative file paths
</commit_message>
<xml_diff>
--- a/Current_Release/v0-2A/Parameters_v0-2A_Tarland.xlsx
+++ b/Current_Release/v0-2A/Parameters_v0-2A_Tarland.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\SimplyP\Development\v0-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Leah_JB\SimplyP_Code\SimplyP\Current_Release\v0-2A\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18195" windowHeight="11160" tabRatio="649" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -598,9 +598,6 @@
     <t>Bulk density(kg/m3)</t>
   </si>
   <si>
-    <t>C:\Data\SimplyP_Local\Temp\Output</t>
-  </si>
-  <si>
     <t>Average latitude of the catchment (used in Thornthwaite PET calculation)</t>
   </si>
   <si>
@@ -687,15 +684,6 @@
   <si>
     <t>NC parameter value is assigned within the model according to the type of newly-converted land
 Values can be sourced from (R)USLE literature. Differences in inherent soil erodibility are generally termed the K factor in USLE-related literature.</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Tarland_MetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Observations\Coull_ChemObs.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_Scotland\Observations\Coull_DailyMeanQ.xlsx</t>
   </si>
   <si>
     <t>Q, TDP, PP</t>
@@ -832,6 +820,18 @@
   </si>
   <si>
     <t>Choose from: SS, TDP, PP, TP, Q, SRP (in any order)</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Tarland_MetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Observations\Coull_ChemObs.xlsx</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Tarland_Scotland\Observations\Coull_DailyMeanQ.xlsx</t>
+  </si>
+  <si>
+    <t>..\..\Example_Data\Example_Output</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2543,7 @@
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2554,20 +2554,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.578125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="55.41796875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="31.3671875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="47.41796875" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="20"/>
+    <col min="1" max="1" width="21.59765625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="55.3984375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="47.3984375" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
         <v>91</v>
       </c>
@@ -2589,47 +2589,47 @@
         <v>92</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>210</v>
+        <v>253</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>113</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="26" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>113</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="26" t="s">
         <v>115</v>
       </c>
@@ -2637,18 +2637,18 @@
         <v>116</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>179</v>
+        <v>255</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>176</v>
@@ -2657,7 +2657,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
         <v>104</v>
       </c>
@@ -2671,40 +2671,40 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="26" t="s">
         <v>97</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C10" s="20">
         <v>1</v>
@@ -2713,12 +2713,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>100</v>
@@ -2727,7 +2727,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
         <v>101</v>
       </c>
@@ -2741,31 +2741,31 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="26" t="s">
-        <v>191</v>
-      </c>
       <c r="B14" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="28" t="s">
         <v>142</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="28" t="s">
         <v>140</v>
       </c>
@@ -2793,12 +2793,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="28" t="s">
         <v>131</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>103</v>
@@ -2807,7 +2807,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28" t="s">
         <v>117</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="26" t="s">
         <v>118</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="26" t="s">
         <v>123</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="26" t="s">
         <v>127</v>
       </c>
@@ -2863,21 +2863,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>202</v>
-      </c>
       <c r="D22" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="26" t="s">
         <v>121</v>
       </c>
@@ -2885,13 +2885,13 @@
         <v>122</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="26" t="s">
         <v>133</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="26" t="s">
         <v>136</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>139</v>
       </c>
@@ -2927,10 +2927,10 @@
         <v>146</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2947,25 +2947,25 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.3125" customWidth="1"/>
-    <col min="3" max="3" width="28.68359375" customWidth="1"/>
+    <col min="1" max="1" width="5.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="139" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" s="139" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" s="139" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2985,18 +2985,18 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.15625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.68359375" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15625" style="17"/>
-    <col min="4" max="4" width="61.7890625" style="17" customWidth="1"/>
-    <col min="5" max="8" width="9.15625" style="17"/>
-    <col min="9" max="9" width="51.15625" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9.15625" style="17"/>
+    <col min="1" max="1" width="11.1328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="17"/>
+    <col min="4" max="4" width="61.796875" style="17" customWidth="1"/>
+    <col min="5" max="8" width="9.1328125" style="17"/>
+    <col min="9" max="9" width="51.1328125" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="62" t="s">
         <v>60</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="67" t="s">
         <v>61</v>
       </c>
@@ -3047,10 +3047,10 @@
       <c r="G2" s="70"/>
       <c r="H2" s="71"/>
       <c r="I2" s="97" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="78" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="73" t="s">
         <v>150</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E3" s="135">
         <v>1458</v>
@@ -3072,10 +3072,10 @@
       <c r="G3" s="76"/>
       <c r="H3" s="77"/>
       <c r="I3" s="98" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="78" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="79" t="s">
         <v>150</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E4" s="137">
         <v>10</v>
@@ -3099,10 +3099,10 @@
         <v>-5</v>
       </c>
       <c r="I4" s="99" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="85" t="s">
         <v>150</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E5" s="138">
         <v>0.1</v>
@@ -3124,10 +3124,10 @@
       <c r="G5" s="89"/>
       <c r="H5" s="90"/>
       <c r="I5" s="100" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="95" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="95" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="91" t="s">
         <v>63</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="91">
         <v>0.2</v>
@@ -3151,10 +3151,10 @@
       </c>
       <c r="H6" s="94"/>
       <c r="I6" s="101" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="172" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="172" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A7" s="173" t="s">
         <v>63</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="175" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E7" s="173">
         <v>0</v>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="H7" s="96"/>
       <c r="I7" s="176" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3195,16 +3195,16 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.15625" style="144" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83984375" style="144" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83984375" style="144"/>
-    <col min="4" max="4" width="58.89453125" style="144" customWidth="1"/>
-    <col min="5" max="16384" width="8.83984375" style="144"/>
+    <col min="1" max="1" width="12.1328125" style="144" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" style="144" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" style="144"/>
+    <col min="4" max="4" width="58.86328125" style="144" customWidth="1"/>
+    <col min="5" max="16384" width="8.86328125" style="144"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="143" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" s="143" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="143" t="s">
         <v>60</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="144" t="s">
         <v>64</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>51.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="144" t="s">
         <v>64</v>
       </c>
@@ -3249,13 +3249,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E3" s="147">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="144" t="s">
         <v>64</v>
       </c>
@@ -3266,13 +3266,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="146" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E4" s="147">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="144" t="s">
         <v>64</v>
       </c>
@@ -3283,13 +3283,13 @@
         <v>17</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E5" s="147">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="177" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" s="177" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="177" t="s">
         <v>64</v>
       </c>
@@ -3300,13 +3300,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="179" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E6" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="177" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" s="177" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="177" t="s">
         <v>64</v>
       </c>
@@ -3317,13 +3317,13 @@
         <v>17</v>
       </c>
       <c r="D7" s="179" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E7" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="177" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" s="177" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="177" t="s">
         <v>64</v>
       </c>
@@ -3334,13 +3334,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="179" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E8" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="92" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" s="92" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="92" t="s">
         <v>63</v>
       </c>
@@ -3351,13 +3351,13 @@
         <v>17</v>
       </c>
       <c r="D9" s="93" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E9" s="147">
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="92" t="s">
         <v>63</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="92" t="s">
         <v>63</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="92" t="s">
         <v>63</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="149" t="s">
         <v>61</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="92" t="s">
         <v>63</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="86" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" s="86" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="86" t="s">
         <v>62</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E15" s="151">
         <v>0.1</v>
@@ -3473,18 +3473,18 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.15625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15625" style="5"/>
-    <col min="4" max="4" width="64.5234375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.15625" style="5"/>
-    <col min="6" max="6" width="62.3125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.15625" style="5"/>
+    <col min="1" max="1" width="12.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="5"/>
+    <col min="4" max="4" width="64.53125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.1328125" style="5"/>
+    <col min="6" max="6" width="62.33203125" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>60</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="181" t="s">
         <v>85</v>
       </c>
@@ -3521,10 +3521,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="184" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="185" t="s">
         <v>85</v>
       </c>
@@ -3541,30 +3541,30 @@
         <v>2.74</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="181" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" s="182" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="183" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="182">
         <v>59.596699999999998</v>
       </c>
       <c r="F4" s="184" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="47" t="s">
         <v>61</v>
       </c>
@@ -3575,14 +3575,14 @@
         <v>17</v>
       </c>
       <c r="D5" s="153" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E5" s="141">
         <v>0.02</v>
       </c>
       <c r="F5" s="49"/>
     </row>
-    <row r="6" spans="1:7" s="118" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" s="118" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="115" t="s">
         <v>61</v>
       </c>
@@ -3593,16 +3593,16 @@
         <v>17</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E6" s="171">
         <v>1</v>
       </c>
       <c r="F6" s="117" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="47" t="s">
         <v>61</v>
       </c>
@@ -3613,16 +3613,16 @@
         <v>12</v>
       </c>
       <c r="D7" s="153" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E7" s="140">
         <v>290</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="47" t="s">
         <v>61</v>
       </c>
@@ -3633,14 +3633,14 @@
         <v>17</v>
       </c>
       <c r="D8" s="153" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E8" s="141">
         <v>0.7</v>
       </c>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="47" t="s">
         <v>61</v>
       </c>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="F9" s="49"/>
     </row>
-    <row r="10" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="47" t="s">
         <v>61</v>
       </c>
@@ -3675,10 +3675,10 @@
         <v>0.4</v>
       </c>
       <c r="F10" s="49" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="47" t="s">
         <v>61</v>
       </c>
@@ -3695,10 +3695,10 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="56" t="s">
         <v>61</v>
       </c>
@@ -3715,10 +3715,10 @@
         <v>0.42</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="47" t="s">
         <v>61</v>
       </c>
@@ -3729,40 +3729,40 @@
         <v>52</v>
       </c>
       <c r="D13" s="153" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13" s="132">
         <v>1</v>
       </c>
       <c r="F13" s="188" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G13" s="114"/>
     </row>
-    <row r="14" spans="1:7" s="124" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" s="124" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="119" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="156" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E14" s="121">
         <v>1</v>
       </c>
       <c r="F14" s="122" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G14" s="123"/>
     </row>
-    <row r="15" spans="1:7" s="128" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" s="128" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A15" s="125" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B15" s="126" t="s">
         <v>32</v>
@@ -3771,18 +3771,18 @@
         <v>53</v>
       </c>
       <c r="D15" s="157" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E15" s="161">
         <v>95</v>
       </c>
       <c r="F15" s="127" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="128" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="129" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B16" s="130" t="s">
         <v>9</v>
@@ -3791,18 +3791,18 @@
         <v>59</v>
       </c>
       <c r="D16" s="158" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E16" s="162">
         <v>1.1315280460000001E-4</v>
       </c>
       <c r="F16" s="131" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="189" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B17" s="190" t="s">
         <v>30</v>
@@ -3818,29 +3818,29 @@
       </c>
       <c r="F17" s="164"/>
     </row>
-    <row r="18" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="189" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B18" s="190" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" s="190" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="163" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" s="165">
         <v>0.7</v>
       </c>
       <c r="F18" s="164" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="192" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="192" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="196" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B19" s="193" t="s">
         <v>31</v>
@@ -3849,14 +3849,14 @@
         <v>17</v>
       </c>
       <c r="D19" s="194" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E19" s="195">
         <v>1.6</v>
       </c>
       <c r="F19" s="113"/>
     </row>
-    <row r="20" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="50" t="s">
         <v>63</v>
       </c>
@@ -3867,14 +3867,14 @@
         <v>16</v>
       </c>
       <c r="D20" s="159" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E20" s="142">
         <v>1500</v>
       </c>
       <c r="F20" s="53"/>
     </row>
-    <row r="21" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="50" t="s">
         <v>63</v>
       </c>
@@ -3885,14 +3885,14 @@
         <v>17</v>
       </c>
       <c r="D21" s="159" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E21" s="169">
         <v>2</v>
       </c>
       <c r="F21" s="53"/>
     </row>
-    <row r="22" spans="1:6" s="52" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" s="52" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="166" t="s">
         <v>63</v>
       </c>
@@ -3909,10 +3909,10 @@
         <v>60</v>
       </c>
       <c r="F22" s="170" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="54" t="s">
         <v>63</v>
       </c>
@@ -3946,35 +3946,35 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.26171875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.41796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.83984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.3984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.15625" style="2"/>
+    <col min="9" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="61">
         <v>7.4999999999999993E-5</v>
       </c>
@@ -3997,12 +3997,12 @@
         <v>4.0175999999999989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>0.01</v>
       </c>
@@ -4038,12 +4038,12 @@
         <v>2.3328000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:6" ht="16.899999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="41" t="s">
         <v>151</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A15" s="34" t="s">
         <v>169</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A16" s="36" t="s">
         <v>54</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="38" t="s">
         <v>55</v>
       </c>
@@ -4124,12 +4124,12 @@
       </c>
       <c r="F17" s="44"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="42.3" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" ht="41.65" x14ac:dyDescent="0.4">
       <c r="A20" s="110" t="s">
         <v>155</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="103" t="s">
         <v>157</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="103" t="s">
         <v>158</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="103" t="s">
         <v>159</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="103" t="s">
         <v>160</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="103" t="s">
         <v>160</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="103" t="s">
         <v>161</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="103" t="s">
         <v>162</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="103" t="s">
         <v>163</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="103" t="s">
         <v>164</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="103" t="s">
         <v>165</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="107" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Small improvements and bug fixes
inputs.py: Added some error checking
model.py: Small bug fixes/improvements;  limit EPC0, Plab and TDPs so they don't go negative; small changes so runs in Python 3 (returning iterators)
visualise_results.py: Add plot for C_cover factor (terrestrial compartment)
</commit_message>
<xml_diff>
--- a/Current_Release/v0-2A/Parameters_v0-2A_Tarland.xlsx
+++ b/Current_Release/v0-2A/Parameters_v0-2A_Tarland.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Leah_JB\SimplyP_Code\SimplyP\Current_Release\v0-2A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\SimplyP\Current_Release\v0-2A\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="690" windowWidth="18195" windowHeight="11160" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18198" windowHeight="11160" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -686,18 +686,10 @@
 Values can be sourced from (R)USLE literature. Differences in inherent soil erodibility are generally termed the K factor in USLE-related literature.</t>
   </si>
   <si>
-    <t>Q, TDP, PP</t>
-  </si>
-  <si>
     <t>2004-01-01</t>
   </si>
   <si>
     <t>2004-12-31</t>
-  </si>
-  <si>
-    <t>One of 'cal', 'other'. Determines:
-- whether Kf is calculated (calibration period) or read in
-- whether observations are plotted (only done for cal &amp; val only)</t>
   </si>
   <si>
     <t>Simulation end date. If calculating PET, must be near 31st December of given year</t>
@@ -725,10 +717,6 @@
 Semi-natural fixed at 0. NC automatically assigned within model</t>
   </si>
   <si>
-    <t>Only supply a value for A.
-Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake and removal</t>
-  </si>
-  <si>
     <t>Proportion of semi-natural and other low soil-P land (value in range 0-1)</t>
   </si>
   <si>
@@ -753,9 +741,6 @@
     <t>Reach effluent TDP inputs. In-stream retention and re-release is not currently taken into account in the model, so if this is important in your catchment you may need to consider this parameter as net inputs after retention</t>
   </si>
   <si>
-    <t>Set to 1 unless PET thought to be systematically under or over-estimated by Thornthwaite in the study area</t>
-  </si>
-  <si>
     <t>Baseflow index (proportion of soil water flow that percolates to groundwater vs flowing to the reach)</t>
   </si>
   <si>
@@ -832,6 +817,21 @@
   </si>
   <si>
     <t>..\..\Example_Data\Example_Output</t>
+  </si>
+  <si>
+    <t>One of 'cal', 'val' or 'scenario'. Determines:
+- whether Kf is calculated (calibration period) or read in. If the latter, then a value for Kf must be supplied in the 'Constant' sheet. This is obtained from calibration.
+- whether observations are plotted (only for cal &amp; val)
+- goodness of fit stats only calculated if not 'scenario'</t>
+  </si>
+  <si>
+    <t>SS, TDP, PP, TP, Q, SRP</t>
+  </si>
+  <si>
+    <t>Only supply a value for A and newly-converted (NC) if any NC land present. Semi-natural fixed at 0. Newly-converted value could be negative if have net uptake and removal</t>
+  </si>
+  <si>
+    <t>Set to 1 unless PET thought to be systematically under or over-estimated in the study area</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1689,6 +1689,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2539,11 +2545,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2554,20 +2560,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="55.3984375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="47.3984375" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="9.1328125" style="20"/>
+    <col min="1" max="1" width="21.578125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="55.41796875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="31.3125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="47.41796875" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="9.1015625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26" t="s">
         <v>91</v>
       </c>
@@ -2589,13 +2595,13 @@
         <v>92</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="26" t="s">
         <v>93</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>197</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>113</v>
@@ -2612,7 +2618,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="26" t="s">
         <v>94</v>
       </c>
@@ -2620,7 +2626,7 @@
         <v>198</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>113</v>
@@ -2629,7 +2635,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="26" t="s">
         <v>115</v>
       </c>
@@ -2637,18 +2643,18 @@
         <v>116</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>176</v>
@@ -2657,7 +2663,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="26" t="s">
         <v>104</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="26" t="s">
         <v>96</v>
       </c>
@@ -2679,32 +2685,32 @@
         <v>181</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="26" t="s">
         <v>97</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C10" s="20">
         <v>1</v>
@@ -2713,21 +2719,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="26" t="s">
         <v>101</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="26" t="s">
         <v>188</v>
       </c>
@@ -2753,7 +2759,7 @@
       </c>
       <c r="D13" s="30"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="26" t="s">
         <v>190</v>
       </c>
@@ -2765,7 +2771,7 @@
       </c>
       <c r="D14" s="30"/>
     </row>
-    <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="28" t="s">
         <v>142</v>
       </c>
@@ -2773,13 +2779,13 @@
         <v>143</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="28" t="s">
         <v>140</v>
       </c>
@@ -2787,13 +2793,13 @@
         <v>141</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="19" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="28" t="s">
         <v>131</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="28" t="s">
         <v>117</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="26" t="s">
         <v>118</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="26" t="s">
         <v>123</v>
       </c>
@@ -2849,7 +2855,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="26" t="s">
         <v>127</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="26" t="s">
         <v>132</v>
       </c>
@@ -2877,7 +2883,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="26" t="s">
         <v>121</v>
       </c>
@@ -2885,13 +2891,13 @@
         <v>122</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>208</v>
+        <v>253</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="26" t="s">
         <v>133</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="26" t="s">
         <v>136</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12" t="s">
         <v>139</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>146</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D26" s="33" t="s">
         <v>187</v>
@@ -2944,17 +2950,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.3125" customWidth="1"/>
+    <col min="3" max="3" width="28.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="139" t="s">
         <v>192</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2982,21 +2988,21 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="17"/>
-    <col min="4" max="4" width="61.796875" style="17" customWidth="1"/>
-    <col min="5" max="8" width="9.1328125" style="17"/>
-    <col min="9" max="9" width="51.1328125" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="17"/>
+    <col min="1" max="1" width="11.1015625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.68359375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1015625" style="17"/>
+    <col min="4" max="4" width="61.7890625" style="17" customWidth="1"/>
+    <col min="5" max="8" width="9.1015625" style="17"/>
+    <col min="9" max="9" width="51.1015625" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="9.1015625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="62" t="s">
         <v>60</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" s="72" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="67" t="s">
         <v>61</v>
       </c>
@@ -3047,10 +3053,10 @@
       <c r="G2" s="70"/>
       <c r="H2" s="71"/>
       <c r="I2" s="97" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="78" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="73" t="s">
         <v>150</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E3" s="135">
         <v>1458</v>
@@ -3072,10 +3078,10 @@
       <c r="G3" s="76"/>
       <c r="H3" s="77"/>
       <c r="I3" s="98" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="78" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="79" t="s">
         <v>150</v>
       </c>
@@ -3086,7 +3092,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E4" s="137">
         <v>10</v>
@@ -3096,13 +3102,13 @@
       </c>
       <c r="G4" s="83"/>
       <c r="H4" s="84">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="99" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.25" customHeight="1" x14ac:dyDescent="0.45">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="78" customFormat="1" ht="61.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="85" t="s">
         <v>150</v>
       </c>
@@ -3113,7 +3119,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E5" s="138">
         <v>0.1</v>
@@ -3124,10 +3130,10 @@
       <c r="G5" s="89"/>
       <c r="H5" s="90"/>
       <c r="I5" s="100" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="95" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="95" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="91" t="s">
         <v>63</v>
       </c>
@@ -3154,7 +3160,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="172" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" s="172" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="173" t="s">
         <v>63</v>
       </c>
@@ -3165,7 +3171,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="175" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E7" s="173">
         <v>0</v>
@@ -3191,20 +3197,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" style="144" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.86328125" style="144" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.86328125" style="144"/>
-    <col min="4" max="4" width="58.86328125" style="144" customWidth="1"/>
-    <col min="5" max="16384" width="8.86328125" style="144"/>
+    <col min="1" max="1" width="12.1015625" style="144" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83984375" style="144" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" style="144"/>
+    <col min="4" max="4" width="58.83984375" style="144" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="144"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="143" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="143" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="143" t="s">
         <v>60</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="144" t="s">
         <v>64</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>51.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="144" t="s">
         <v>64</v>
       </c>
@@ -3249,13 +3255,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="146" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E3" s="147">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="144" t="s">
         <v>64</v>
       </c>
@@ -3266,13 +3272,13 @@
         <v>17</v>
       </c>
       <c r="D4" s="146" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E4" s="147">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="144" t="s">
         <v>64</v>
       </c>
@@ -3283,13 +3289,13 @@
         <v>17</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E5" s="147">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="177" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" s="177" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="177" t="s">
         <v>64</v>
       </c>
@@ -3300,13 +3306,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="179" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E6" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="177" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" s="177" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="177" t="s">
         <v>64</v>
       </c>
@@ -3317,13 +3323,13 @@
         <v>17</v>
       </c>
       <c r="D7" s="179" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E7" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="177" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="177" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="177" t="s">
         <v>64</v>
       </c>
@@ -3334,30 +3340,30 @@
         <v>17</v>
       </c>
       <c r="D8" s="179" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E8" s="180">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="92" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A9" s="92" t="s">
+    <row r="9" spans="1:5" s="197" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="197" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="197" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="93" t="s">
-        <v>227</v>
-      </c>
-      <c r="E9" s="147">
+      <c r="D9" s="198" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" s="180">
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="92" t="s">
         <v>63</v>
       </c>
@@ -3374,7 +3380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="92" t="s">
         <v>63</v>
       </c>
@@ -3391,7 +3397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="92" t="s">
         <v>63</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" s="149" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="149" t="s">
         <v>61</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="92" t="s">
         <v>63</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="86" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" s="86" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="86" t="s">
         <v>62</v>
       </c>
@@ -3453,7 +3459,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E15" s="151">
         <v>0.1</v>
@@ -3469,22 +3475,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="5"/>
-    <col min="4" max="4" width="64.53125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" style="5"/>
-    <col min="6" max="6" width="62.33203125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.1328125" style="5"/>
+    <col min="1" max="1" width="12.1015625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.68359375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1015625" style="5"/>
+    <col min="4" max="4" width="64.5234375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.1015625" style="5"/>
+    <col min="6" max="6" width="62.3125" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1015625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
         <v>60</v>
       </c>
@@ -3504,7 +3510,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="181" t="s">
         <v>85</v>
       </c>
@@ -3521,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="184" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="185" t="s">
         <v>85</v>
       </c>
@@ -3541,10 +3547,10 @@
         <v>2.74</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="181" t="s">
         <v>61</v>
       </c>
@@ -3561,10 +3567,10 @@
         <v>59.596699999999998</v>
       </c>
       <c r="F4" s="184" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="47" t="s">
         <v>61</v>
       </c>
@@ -3575,14 +3581,14 @@
         <v>17</v>
       </c>
       <c r="D5" s="153" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E5" s="141">
         <v>0.02</v>
       </c>
       <c r="F5" s="49"/>
     </row>
-    <row r="6" spans="1:7" s="118" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="118" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="115" t="s">
         <v>61</v>
       </c>
@@ -3593,16 +3599,16 @@
         <v>17</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E6" s="171">
         <v>1</v>
       </c>
       <c r="F6" s="117" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="47" t="s">
         <v>61</v>
       </c>
@@ -3613,16 +3619,16 @@
         <v>12</v>
       </c>
       <c r="D7" s="153" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E7" s="140">
         <v>290</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="47" t="s">
         <v>61</v>
       </c>
@@ -3633,14 +3639,14 @@
         <v>17</v>
       </c>
       <c r="D8" s="153" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E8" s="141">
         <v>0.7</v>
       </c>
       <c r="F8" s="49"/>
     </row>
-    <row r="9" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="47" t="s">
         <v>61</v>
       </c>
@@ -3658,7 +3664,7 @@
       </c>
       <c r="F9" s="49"/>
     </row>
-    <row r="10" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="47" t="s">
         <v>61</v>
       </c>
@@ -3675,10 +3681,10 @@
         <v>0.4</v>
       </c>
       <c r="F10" s="49" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.45">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="47" t="s">
         <v>61</v>
       </c>
@@ -3695,10 +3701,10 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="60" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="56" t="s">
         <v>61</v>
       </c>
@@ -3715,10 +3721,10 @@
         <v>0.42</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="46" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="47" t="s">
         <v>61</v>
       </c>
@@ -3735,11 +3741,11 @@
         <v>1</v>
       </c>
       <c r="F13" s="188" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G13" s="114"/>
     </row>
-    <row r="14" spans="1:7" s="124" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" s="124" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="119" t="s">
         <v>61</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="156" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E14" s="121">
         <v>1</v>
@@ -3760,9 +3766,9 @@
       </c>
       <c r="G14" s="123"/>
     </row>
-    <row r="15" spans="1:7" s="128" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" s="128" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="125" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B15" s="126" t="s">
         <v>32</v>
@@ -3777,12 +3783,12 @@
         <v>95</v>
       </c>
       <c r="F15" s="127" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="128" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="129" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B16" s="130" t="s">
         <v>9</v>
@@ -3791,7 +3797,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="158" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E16" s="162">
         <v>1.1315280460000001E-4</v>
@@ -3800,9 +3806,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="189" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B17" s="190" t="s">
         <v>30</v>
@@ -3818,9 +3824,9 @@
       </c>
       <c r="F17" s="164"/>
     </row>
-    <row r="18" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" s="192" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="189" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B18" s="190" t="s">
         <v>186</v>
@@ -3838,9 +3844,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="192" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" s="192" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="196" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B19" s="193" t="s">
         <v>31</v>
@@ -3849,14 +3855,14 @@
         <v>17</v>
       </c>
       <c r="D19" s="194" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E19" s="195">
         <v>1.6</v>
       </c>
       <c r="F19" s="113"/>
     </row>
-    <row r="20" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="50" t="s">
         <v>63</v>
       </c>
@@ -3867,14 +3873,14 @@
         <v>16</v>
       </c>
       <c r="D20" s="159" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E20" s="142">
         <v>1500</v>
       </c>
       <c r="F20" s="53"/>
     </row>
-    <row r="21" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="50" t="s">
         <v>63</v>
       </c>
@@ -3885,14 +3891,14 @@
         <v>17</v>
       </c>
       <c r="D21" s="159" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E21" s="169">
         <v>2</v>
       </c>
       <c r="F21" s="53"/>
     </row>
-    <row r="22" spans="1:6" s="52" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" s="52" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="166" t="s">
         <v>63</v>
       </c>
@@ -3909,10 +3915,10 @@
         <v>60</v>
       </c>
       <c r="F22" s="170" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.45">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="54" t="s">
         <v>63</v>
       </c>
@@ -3946,35 +3952,35 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.26171875" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.3984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.26171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.41796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83984375" style="2" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="2"/>
+    <col min="9" max="16384" width="9.1015625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="61">
         <v>7.4999999999999993E-5</v>
       </c>
@@ -3997,12 +4003,12 @@
         <v>4.0175999999999989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
@@ -4019,7 +4025,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
         <v>0.01</v>
       </c>
@@ -4038,12 +4044,12 @@
         <v>2.3328000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.899999999999999" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.65">
       <c r="A13" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="41" t="s">
         <v>151</v>
       </c>
@@ -4063,7 +4069,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
       <c r="A15" s="34" t="s">
         <v>169</v>
       </c>
@@ -4083,7 +4089,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="28.2" x14ac:dyDescent="0.5">
       <c r="A16" s="36" t="s">
         <v>54</v>
       </c>
@@ -4103,7 +4109,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="38" t="s">
         <v>55</v>
       </c>
@@ -4124,12 +4130,12 @@
       </c>
       <c r="F17" s="44"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="41.65" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="42.3" x14ac:dyDescent="0.5">
       <c r="A20" s="110" t="s">
         <v>155</v>
       </c>
@@ -4140,7 +4146,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="103" t="s">
         <v>157</v>
       </c>
@@ -4152,7 +4158,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="103" t="s">
         <v>158</v>
       </c>
@@ -4164,7 +4170,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="103" t="s">
         <v>159</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="103" t="s">
         <v>160</v>
       </c>
@@ -4188,7 +4194,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="103" t="s">
         <v>160</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="103" t="s">
         <v>161</v>
       </c>
@@ -4212,7 +4218,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="103" t="s">
         <v>162</v>
       </c>
@@ -4224,7 +4230,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="103" t="s">
         <v>163</v>
       </c>
@@ -4236,7 +4242,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="103" t="s">
         <v>164</v>
       </c>
@@ -4248,7 +4254,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="103" t="s">
         <v>165</v>
       </c>
@@ -4260,7 +4266,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="107" t="s">
         <v>166</v>
       </c>

</xml_diff>